<commit_message>
Adding 2nd level division sheet
</commit_message>
<xml_diff>
--- a/PrintSheets.xlsx
+++ b/PrintSheets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1110" yWindow="2295" windowWidth="18000" windowHeight="9360" tabRatio="600" firstSheet="3" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Addition" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,12 +11,14 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Simple Multiplication" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Simple Division" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2nd level Multiplication" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2nd level Division" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Addition'!$A$1:$K$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Subtraction'!$A$1:$K$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Simple Multiplication'!$A$1:$K$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Simple Division'!$A$1:$K$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'2nd level Division'!$A$1:$K$23</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -84,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -139,11 +141,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -180,6 +191,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,19 +541,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="8" min="6" max="6"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="8" min="9" max="9"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="8" min="12" max="22"/>
-    <col width="12.140625" customWidth="1" style="8" min="23" max="16384"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="1" max="1"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="4" max="4"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="7" max="7"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
+    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1036,19 +1056,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="8" min="6" max="6"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="8" min="9" max="9"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="8" min="12" max="22"/>
-    <col width="12.140625" customWidth="1" style="8" min="23" max="16384"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="1" max="1"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="4" max="4"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="7" max="7"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
+    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1551,19 +1571,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="8" min="6" max="6"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="8" min="9" max="9"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="8" min="12" max="22"/>
-    <col width="12.140625" customWidth="1" style="8" min="23" max="16384"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="1" max="1"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="4" max="4"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="7" max="7"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
+    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -2060,39 +2080,39 @@
   </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="8" min="6" max="6"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="8" min="9" max="9"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="8" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="8" min="12" max="22"/>
-    <col width="12.140625" customWidth="1" style="8" min="23" max="16384"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="1" max="1"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="4" max="4"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="7" max="7"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
+    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
       <c r="B1" s="1" t="n">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1" t="n">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
@@ -2102,7 +2122,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
@@ -2110,44 +2130,44 @@
         </is>
       </c>
       <c r="E2" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>÷</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="J2" s="2" t="inlineStr">
         <is>
           <t>÷</t>
         </is>
       </c>
-      <c r="H2" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>÷</t>
-        </is>
-      </c>
       <c r="K2" s="3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" ht="21.75" customHeight="1" thickBot="1">
       <c r="A3" s="4" t="n"/>
       <c r="B3" s="5" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="n"/>
       <c r="D3" s="4" t="n"/>
       <c r="E3" s="5" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F3" s="4" t="n"/>
       <c r="G3" s="4" t="n"/>
       <c r="H3" s="5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I3" s="4" t="n"/>
       <c r="J3" s="4" t="n"/>
       <c r="K3" s="5" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" thickTop="1">
@@ -2168,13 +2188,13 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" ht="20.25" customHeight="1">
@@ -2192,7 +2212,7 @@
         </is>
       </c>
       <c r="E6" s="3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -2200,7 +2220,7 @@
         </is>
       </c>
       <c r="H6" s="3" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
@@ -2208,7 +2228,7 @@
         </is>
       </c>
       <c r="K6" s="3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" ht="21.75" customHeight="1" thickBot="1">
@@ -2219,17 +2239,17 @@
       <c r="C7" s="4" t="n"/>
       <c r="D7" s="4" t="n"/>
       <c r="E7" s="5" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F7" s="4" t="n"/>
       <c r="G7" s="4" t="n"/>
       <c r="H7" s="5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I7" s="4" t="n"/>
       <c r="J7" s="4" t="n"/>
       <c r="K7" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" thickTop="1">
@@ -2247,16 +2267,16 @@
     </row>
     <row r="9" ht="20.25" customHeight="1">
       <c r="B9" s="1" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>15</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" ht="20.25" customHeight="1">
@@ -2266,7 +2286,7 @@
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
@@ -2274,7 +2294,7 @@
         </is>
       </c>
       <c r="E10" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
@@ -2282,7 +2302,7 @@
         </is>
       </c>
       <c r="H10" s="3" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -2290,18 +2310,18 @@
         </is>
       </c>
       <c r="K10" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" ht="21.75" customHeight="1" thickBot="1">
       <c r="A11" s="4" t="n"/>
       <c r="B11" s="5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C11" s="4" t="n"/>
       <c r="D11" s="4" t="n"/>
       <c r="E11" s="5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="4" t="n"/>
       <c r="G11" s="4" t="n"/>
@@ -2311,7 +2331,7 @@
       <c r="I11" s="4" t="n"/>
       <c r="J11" s="4" t="n"/>
       <c r="K11" s="5" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" thickTop="1">
@@ -2329,16 +2349,16 @@
     </row>
     <row r="13" ht="20.25" customHeight="1">
       <c r="B13" s="1" t="n">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" ht="20.25" customHeight="1">
@@ -2348,7 +2368,7 @@
         </is>
       </c>
       <c r="B14" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
@@ -2364,7 +2384,7 @@
         </is>
       </c>
       <c r="H14" s="3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J14" s="2" t="inlineStr">
         <is>
@@ -2372,28 +2392,28 @@
         </is>
       </c>
       <c r="K14" s="3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" ht="21.75" customHeight="1" thickBot="1">
       <c r="A15" s="4" t="n"/>
       <c r="B15" s="5" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C15" s="4" t="n"/>
       <c r="D15" s="4" t="n"/>
       <c r="E15" s="5" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F15" s="4" t="n"/>
       <c r="G15" s="4" t="n"/>
       <c r="H15" s="5" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I15" s="4" t="n"/>
       <c r="J15" s="4" t="n"/>
       <c r="K15" s="5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" thickTop="1">
@@ -2411,16 +2431,16 @@
     </row>
     <row r="17" ht="20.25" customHeight="1">
       <c r="B17" s="1" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" ht="20.25" customHeight="1">
@@ -2430,7 +2450,7 @@
         </is>
       </c>
       <c r="B18" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
@@ -2446,7 +2466,7 @@
         </is>
       </c>
       <c r="H18" s="3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J18" s="2" t="inlineStr">
         <is>
@@ -2454,28 +2474,28 @@
         </is>
       </c>
       <c r="K18" s="3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" ht="21.75" customHeight="1" thickBot="1">
       <c r="A19" s="4" t="n"/>
       <c r="B19" s="5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" s="4" t="n"/>
       <c r="D19" s="4" t="n"/>
       <c r="E19" s="5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" s="4" t="n"/>
       <c r="G19" s="4" t="n"/>
       <c r="H19" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I19" s="4" t="n"/>
       <c r="J19" s="4" t="n"/>
       <c r="K19" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" thickTop="1">
@@ -2493,16 +2513,16 @@
     </row>
     <row r="21" ht="20.25" customHeight="1">
       <c r="B21" s="1" t="n">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="H21" s="1" t="n">
+      <c r="K21" s="1" t="n">
         <v>48</v>
-      </c>
-      <c r="K21" s="1" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="22" ht="20.25" customHeight="1">
@@ -2512,7 +2532,7 @@
         </is>
       </c>
       <c r="B22" s="3" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
@@ -2528,7 +2548,7 @@
         </is>
       </c>
       <c r="H22" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J22" s="2" t="inlineStr">
         <is>
@@ -2542,22 +2562,22 @@
     <row r="23" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="4" t="n"/>
       <c r="B23" s="5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C23" s="4" t="n"/>
       <c r="D23" s="4" t="n"/>
       <c r="E23" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F23" s="4" t="n"/>
       <c r="G23" s="4" t="n"/>
       <c r="H23" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I23" s="4" t="n"/>
       <c r="J23" s="4" t="n"/>
       <c r="K23" s="5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" ht="21.75" customHeight="1" thickTop="1"/>
@@ -2575,25 +2595,25 @@
   </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
     <col width="5.140625" customWidth="1" style="13" min="1" max="1"/>
-    <col width="6.140625" customWidth="1" style="8" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="6.140625" customWidth="1" style="17" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
     <col width="5.140625" customWidth="1" style="13" min="4" max="4"/>
-    <col width="6.140625" customWidth="1" style="8" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="8" min="6" max="6"/>
+    <col width="6.140625" customWidth="1" style="17" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
     <col width="5.140625" customWidth="1" style="13" min="7" max="7"/>
-    <col width="6.140625" customWidth="1" style="8" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="8" min="9" max="9"/>
+    <col width="6.140625" customWidth="1" style="17" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
     <col width="5.140625" customWidth="1" style="13" min="10" max="10"/>
-    <col width="6.140625" customWidth="1" style="8" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="8" min="12" max="22"/>
-    <col width="12.140625" customWidth="1" style="8" min="23" max="16384"/>
+    <col width="6.140625" customWidth="1" style="17" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
+    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -3028,4 +3048,382 @@
   <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.5511811023622047" bottom="0.5511811023622047" header="0.3149606299212598" footer="0.3149606299212598"/>
   <pageSetup orientation="portrait" paperSize="9" scale="160"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
+  <cols>
+    <col width="6.140625" customWidth="1" style="17" min="1" max="2"/>
+    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
+    <col width="6.140625" customWidth="1" style="17" min="4" max="5"/>
+    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
+    <col width="6.140625" customWidth="1" style="17" min="7" max="8"/>
+    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
+    <col width="6.140625" customWidth="1" style="17" min="10" max="11"/>
+    <col width="2.85546875" customWidth="1" style="17" min="12" max="12"/>
+    <col width="12.140625" customWidth="1" style="17" min="13" max="24"/>
+    <col width="12.140625" customWidth="1" style="17" min="25" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="J1" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K1" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" s="20" t="n"/>
+      <c r="B2" s="18" t="n"/>
+      <c r="D2" s="20" t="n"/>
+      <c r="E2" s="18" t="n"/>
+      <c r="G2" s="20" t="n"/>
+      <c r="H2" s="18" t="n"/>
+      <c r="J2" s="20" t="n"/>
+      <c r="K2" s="18" t="n"/>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" s="20" t="n"/>
+      <c r="B3" s="19" t="n"/>
+      <c r="D3" s="20" t="n"/>
+      <c r="E3" s="19" t="n"/>
+      <c r="G3" s="20" t="n"/>
+      <c r="H3" s="19" t="n"/>
+      <c r="J3" s="20" t="n"/>
+      <c r="K3" s="19" t="n"/>
+    </row>
+    <row r="4" ht="20.25" customHeight="1">
+      <c r="A4" s="19" t="n"/>
+      <c r="B4" s="19" t="n"/>
+      <c r="C4" s="17" t="n"/>
+      <c r="D4" s="19" t="n"/>
+      <c r="E4" s="19" t="n"/>
+      <c r="F4" s="17" t="n"/>
+      <c r="G4" s="19" t="n"/>
+      <c r="H4" s="19" t="n"/>
+      <c r="I4" s="17" t="n"/>
+      <c r="J4" s="19" t="n"/>
+      <c r="K4" s="19" t="n"/>
+      <c r="L4" s="17" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="J5" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="20" t="n"/>
+      <c r="B6" s="18" t="n"/>
+      <c r="D6" s="20" t="n"/>
+      <c r="E6" s="18" t="n"/>
+      <c r="G6" s="20" t="n"/>
+      <c r="H6" s="18" t="n"/>
+      <c r="J6" s="20" t="n"/>
+      <c r="K6" s="18" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="20" t="n"/>
+      <c r="B7" s="19" t="n"/>
+      <c r="D7" s="20" t="n"/>
+      <c r="E7" s="19" t="n"/>
+      <c r="G7" s="20" t="n"/>
+      <c r="H7" s="19" t="n"/>
+      <c r="J7" s="20" t="n"/>
+      <c r="K7" s="19" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="19" t="n"/>
+      <c r="B8" s="19" t="n"/>
+      <c r="C8" s="17" t="n"/>
+      <c r="D8" s="19" t="n"/>
+      <c r="E8" s="19" t="n"/>
+      <c r="F8" s="17" t="n"/>
+      <c r="G8" s="19" t="n"/>
+      <c r="H8" s="19" t="n"/>
+      <c r="I8" s="17" t="n"/>
+      <c r="J8" s="19" t="n"/>
+      <c r="K8" s="19" t="n"/>
+      <c r="L8" s="17" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J9" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="20" t="n"/>
+      <c r="B10" s="18" t="n"/>
+      <c r="D10" s="20" t="n"/>
+      <c r="E10" s="18" t="n"/>
+      <c r="G10" s="20" t="n"/>
+      <c r="H10" s="18" t="n"/>
+      <c r="J10" s="20" t="n"/>
+      <c r="K10" s="18" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="20" t="n"/>
+      <c r="B11" s="19" t="n"/>
+      <c r="D11" s="20" t="n"/>
+      <c r="E11" s="19" t="n"/>
+      <c r="G11" s="20" t="n"/>
+      <c r="H11" s="19" t="n"/>
+      <c r="J11" s="20" t="n"/>
+      <c r="K11" s="19" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="19" t="n"/>
+      <c r="B12" s="19" t="n"/>
+      <c r="C12" s="17" t="n"/>
+      <c r="D12" s="19" t="n"/>
+      <c r="E12" s="19" t="n"/>
+      <c r="F12" s="17" t="n"/>
+      <c r="G12" s="19" t="n"/>
+      <c r="H12" s="19" t="n"/>
+      <c r="I12" s="17" t="n"/>
+      <c r="J12" s="19" t="n"/>
+      <c r="K12" s="19" t="n"/>
+      <c r="L12" s="17" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="J13" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="20" t="n"/>
+      <c r="B14" s="18" t="n"/>
+      <c r="D14" s="20" t="n"/>
+      <c r="E14" s="18" t="n"/>
+      <c r="G14" s="20" t="n"/>
+      <c r="H14" s="18" t="n"/>
+      <c r="J14" s="20" t="n"/>
+      <c r="K14" s="18" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="20" t="n"/>
+      <c r="B15" s="19" t="n"/>
+      <c r="D15" s="20" t="n"/>
+      <c r="E15" s="19" t="n"/>
+      <c r="G15" s="20" t="n"/>
+      <c r="H15" s="19" t="n"/>
+      <c r="J15" s="20" t="n"/>
+      <c r="K15" s="19" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="19" t="n"/>
+      <c r="B16" s="19" t="n"/>
+      <c r="C16" s="17" t="n"/>
+      <c r="D16" s="19" t="n"/>
+      <c r="E16" s="19" t="n"/>
+      <c r="F16" s="17" t="n"/>
+      <c r="G16" s="19" t="n"/>
+      <c r="H16" s="19" t="n"/>
+      <c r="I16" s="17" t="n"/>
+      <c r="J16" s="19" t="n"/>
+      <c r="K16" s="19" t="n"/>
+      <c r="L16" s="17" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D17" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G17" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J17" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="K17" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="20" t="n"/>
+      <c r="B18" s="18" t="n"/>
+      <c r="D18" s="20" t="n"/>
+      <c r="E18" s="18" t="n"/>
+      <c r="G18" s="20" t="n"/>
+      <c r="H18" s="18" t="n"/>
+      <c r="J18" s="20" t="n"/>
+      <c r="K18" s="18" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="20" t="n"/>
+      <c r="B19" s="19" t="n"/>
+      <c r="D19" s="20" t="n"/>
+      <c r="E19" s="19" t="n"/>
+      <c r="G19" s="20" t="n"/>
+      <c r="H19" s="19" t="n"/>
+      <c r="J19" s="20" t="n"/>
+      <c r="K19" s="19" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="19" t="n"/>
+      <c r="B20" s="19" t="n"/>
+      <c r="C20" s="17" t="n"/>
+      <c r="D20" s="19" t="n"/>
+      <c r="E20" s="19" t="n"/>
+      <c r="F20" s="17" t="n"/>
+      <c r="G20" s="19" t="n"/>
+      <c r="H20" s="19" t="n"/>
+      <c r="I20" s="17" t="n"/>
+      <c r="J20" s="19" t="n"/>
+      <c r="K20" s="19" t="n"/>
+      <c r="L20" s="17" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G21" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J21" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="K21" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="20" t="n"/>
+      <c r="B22" s="18" t="n"/>
+      <c r="D22" s="20" t="n"/>
+      <c r="E22" s="18" t="n"/>
+      <c r="G22" s="20" t="n"/>
+      <c r="H22" s="18" t="n"/>
+      <c r="J22" s="20" t="n"/>
+      <c r="K22" s="18" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="20" t="n"/>
+      <c r="B23" s="19" t="n"/>
+      <c r="D23" s="20" t="n"/>
+      <c r="E23" s="19" t="n"/>
+      <c r="G23" s="20" t="n"/>
+      <c r="H23" s="19" t="n"/>
+      <c r="J23" s="20" t="n"/>
+      <c r="K23" s="19" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.5511811023622047" bottom="0.5511811023622047" header="0.3149606299212598" footer="0.3149606299212598"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="150"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update 2nd level division
</commit_message>
<xml_diff>
--- a/PrintSheets.xlsx
+++ b/PrintSheets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1110" yWindow="2295" windowWidth="18000" windowHeight="9360" tabRatio="600" firstSheet="3" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="600" firstSheet="3" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Addition" sheetId="1" state="visible" r:id="rId1"/>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -173,9 +173,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -541,19 +538,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="1" max="1"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="4" max="4"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="7" max="7"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
-    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="1" max="1"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="16" min="3" max="3"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="4" max="4"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="16" min="6" max="6"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="7" max="7"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="16" min="9" max="9"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="10" max="10"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="16" min="12" max="25"/>
+    <col width="12.140625" customWidth="1" style="16" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1056,19 +1053,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="1" max="1"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="4" max="4"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="7" max="7"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
-    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="1" max="1"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="16" min="3" max="3"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="4" max="4"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="16" min="6" max="6"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="7" max="7"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="16" min="9" max="9"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="10" max="10"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="16" min="12" max="25"/>
+    <col width="12.140625" customWidth="1" style="16" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1571,19 +1568,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="1" max="1"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="4" max="4"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="7" max="7"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
-    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="1" max="1"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="16" min="3" max="3"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="4" max="4"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="16" min="6" max="6"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="7" max="7"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="16" min="9" max="9"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="10" max="10"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="16" min="12" max="25"/>
+    <col width="12.140625" customWidth="1" style="16" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -2086,19 +2083,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="1" max="1"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="4" max="4"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="7" max="7"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
-    <col width="2.7109375" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="17" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
-    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="1" max="1"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="16" min="3" max="3"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="4" max="4"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="16" min="6" max="6"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="7" max="7"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="16" min="9" max="9"/>
+    <col width="2.7109375" bestFit="1" customWidth="1" style="16" min="10" max="10"/>
+    <col width="7.5703125" bestFit="1" customWidth="1" style="16" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="16" min="12" max="25"/>
+    <col width="12.140625" customWidth="1" style="16" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -2601,19 +2598,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="5.140625" customWidth="1" style="13" min="1" max="1"/>
-    <col width="6.140625" customWidth="1" style="17" min="2" max="2"/>
-    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
-    <col width="5.140625" customWidth="1" style="13" min="4" max="4"/>
-    <col width="6.140625" customWidth="1" style="17" min="5" max="5"/>
-    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
-    <col width="5.140625" customWidth="1" style="13" min="7" max="7"/>
-    <col width="6.140625" customWidth="1" style="17" min="8" max="8"/>
-    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
-    <col width="5.140625" customWidth="1" style="13" min="10" max="10"/>
-    <col width="6.140625" customWidth="1" style="17" min="11" max="11"/>
-    <col width="12.140625" customWidth="1" style="17" min="12" max="23"/>
-    <col width="12.140625" customWidth="1" style="17" min="24" max="16384"/>
+    <col width="5.140625" customWidth="1" style="12" min="1" max="1"/>
+    <col width="6.140625" customWidth="1" style="16" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" style="16" min="3" max="3"/>
+    <col width="5.140625" customWidth="1" style="12" min="4" max="4"/>
+    <col width="6.140625" customWidth="1" style="16" min="5" max="5"/>
+    <col width="2.85546875" customWidth="1" style="16" min="6" max="6"/>
+    <col width="5.140625" customWidth="1" style="12" min="7" max="7"/>
+    <col width="6.140625" customWidth="1" style="16" min="8" max="8"/>
+    <col width="2.85546875" customWidth="1" style="16" min="9" max="9"/>
+    <col width="5.140625" customWidth="1" style="12" min="10" max="10"/>
+    <col width="6.140625" customWidth="1" style="16" min="11" max="11"/>
+    <col width="12.140625" customWidth="1" style="16" min="12" max="25"/>
+    <col width="12.140625" customWidth="1" style="16" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -2631,7 +2628,7 @@
       </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="12" t="inlineStr">
+      <c r="A2" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2639,7 +2636,7 @@
       <c r="B2" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="D2" s="12" t="inlineStr">
+      <c r="D2" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2647,7 +2644,7 @@
       <c r="E2" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="G2" s="12" t="inlineStr">
+      <c r="G2" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2655,7 +2652,7 @@
       <c r="H2" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="J2" s="12" t="inlineStr">
+      <c r="J2" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2665,65 +2662,65 @@
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="9" t="n">
+      <c r="E3" s="8" t="n">
         <v>108</v>
       </c>
-      <c r="H3" s="9" t="n">
+      <c r="H3" s="8" t="n">
         <v>127</v>
       </c>
-      <c r="K3" s="9" t="n">
+      <c r="K3" s="8" t="n">
         <v>563</v>
       </c>
     </row>
     <row r="4" ht="20.25" customHeight="1">
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="11" t="n">
+      <c r="E4" s="10" t="n">
         <v>108</v>
       </c>
-      <c r="H4" s="11" t="n">
+      <c r="H4" s="10" t="n">
         <v>127</v>
       </c>
-      <c r="K4" s="11" t="n">
+      <c r="K4" s="10" t="n">
         <v>563</v>
       </c>
     </row>
     <row r="5" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A5" s="14" t="n"/>
-      <c r="B5" s="10" t="n">
+      <c r="A5" s="13" t="n"/>
+      <c r="B5" s="9" t="n">
         <v>913</v>
       </c>
       <c r="C5" s="4" t="n"/>
-      <c r="D5" s="14" t="n"/>
-      <c r="E5" s="10" t="n">
+      <c r="D5" s="13" t="n"/>
+      <c r="E5" s="9" t="n">
         <v>899</v>
       </c>
       <c r="F5" s="4" t="n"/>
-      <c r="G5" s="14" t="n"/>
-      <c r="H5" s="10" t="n">
+      <c r="G5" s="13" t="n"/>
+      <c r="H5" s="9" t="n">
         <v>969</v>
       </c>
       <c r="I5" s="4" t="n"/>
-      <c r="J5" s="14" t="n"/>
-      <c r="K5" s="10" t="n">
+      <c r="J5" s="13" t="n"/>
+      <c r="K5" s="9" t="n">
         <v>660</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A6" s="15" t="n"/>
+      <c r="A6" s="14" t="n"/>
       <c r="B6" s="7" t="n"/>
       <c r="C6" s="6" t="n"/>
-      <c r="D6" s="15" t="n"/>
+      <c r="D6" s="14" t="n"/>
       <c r="E6" s="7" t="n"/>
       <c r="F6" s="6" t="n"/>
-      <c r="G6" s="15" t="n"/>
+      <c r="G6" s="14" t="n"/>
       <c r="H6" s="7" t="n"/>
       <c r="I6" s="6" t="n"/>
-      <c r="J6" s="15" t="n"/>
+      <c r="J6" s="14" t="n"/>
       <c r="K6" s="7" t="n"/>
     </row>
     <row r="7" ht="20.25" customHeight="1">
@@ -2741,7 +2738,7 @@
       </c>
     </row>
     <row r="8" ht="20.25" customHeight="1">
-      <c r="A8" s="12" t="inlineStr">
+      <c r="A8" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2749,7 +2746,7 @@
       <c r="B8" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="D8" s="12" t="inlineStr">
+      <c r="D8" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2757,7 +2754,7 @@
       <c r="E8" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="G8" s="12" t="inlineStr">
+      <c r="G8" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2765,7 +2762,7 @@
       <c r="H8" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="J8" s="12" t="inlineStr">
+      <c r="J8" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2775,65 +2772,65 @@
       </c>
     </row>
     <row r="9" ht="20.25" customHeight="1">
-      <c r="B9" s="9" t="n">
+      <c r="B9" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="E9" s="9" t="n">
+      <c r="E9" s="8" t="n">
         <v>108</v>
       </c>
-      <c r="H9" s="9" t="n">
+      <c r="H9" s="8" t="n">
         <v>127</v>
       </c>
-      <c r="K9" s="9" t="n">
+      <c r="K9" s="8" t="n">
         <v>563</v>
       </c>
     </row>
     <row r="10" ht="20.25" customHeight="1">
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="E10" s="11" t="n">
+      <c r="E10" s="10" t="n">
         <v>108</v>
       </c>
-      <c r="H10" s="11" t="n">
+      <c r="H10" s="10" t="n">
         <v>127</v>
       </c>
-      <c r="K10" s="11" t="n">
+      <c r="K10" s="10" t="n">
         <v>563</v>
       </c>
     </row>
     <row r="11" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="10" t="n">
+      <c r="A11" s="13" t="n"/>
+      <c r="B11" s="9" t="n">
         <v>390</v>
       </c>
       <c r="C11" s="4" t="n"/>
-      <c r="D11" s="14" t="n"/>
-      <c r="E11" s="10" t="n">
+      <c r="D11" s="13" t="n"/>
+      <c r="E11" s="9" t="n">
         <v>782</v>
       </c>
       <c r="F11" s="4" t="n"/>
-      <c r="G11" s="14" t="n"/>
-      <c r="H11" s="10" t="n">
+      <c r="G11" s="13" t="n"/>
+      <c r="H11" s="9" t="n">
         <v>459</v>
       </c>
       <c r="I11" s="4" t="n"/>
-      <c r="J11" s="14" t="n"/>
-      <c r="K11" s="10" t="n">
+      <c r="J11" s="13" t="n"/>
+      <c r="K11" s="9" t="n">
         <v>280</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A12" s="15" t="n"/>
+      <c r="A12" s="14" t="n"/>
       <c r="B12" s="7" t="n"/>
       <c r="C12" s="6" t="n"/>
-      <c r="D12" s="15" t="n"/>
+      <c r="D12" s="14" t="n"/>
       <c r="E12" s="7" t="n"/>
       <c r="F12" s="6" t="n"/>
-      <c r="G12" s="15" t="n"/>
+      <c r="G12" s="14" t="n"/>
       <c r="H12" s="7" t="n"/>
       <c r="I12" s="6" t="n"/>
-      <c r="J12" s="15" t="n"/>
+      <c r="J12" s="14" t="n"/>
       <c r="K12" s="7" t="n"/>
     </row>
     <row r="13" ht="20.25" customHeight="1">
@@ -2851,7 +2848,7 @@
       </c>
     </row>
     <row r="14" ht="20.25" customHeight="1">
-      <c r="A14" s="12" t="inlineStr">
+      <c r="A14" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2859,7 +2856,7 @@
       <c r="B14" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="D14" s="12" t="inlineStr">
+      <c r="D14" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2867,7 +2864,7 @@
       <c r="E14" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="G14" s="12" t="inlineStr">
+      <c r="G14" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2875,7 +2872,7 @@
       <c r="H14" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="J14" s="12" t="inlineStr">
+      <c r="J14" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2885,65 +2882,65 @@
       </c>
     </row>
     <row r="15" ht="20.25" customHeight="1">
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="E15" s="9" t="n">
+      <c r="E15" s="8" t="n">
         <v>108</v>
       </c>
-      <c r="H15" s="9" t="n">
+      <c r="H15" s="8" t="n">
         <v>127</v>
       </c>
-      <c r="K15" s="9" t="n">
+      <c r="K15" s="8" t="n">
         <v>563</v>
       </c>
     </row>
     <row r="16" ht="20.25" customHeight="1">
-      <c r="B16" s="11" t="n">
+      <c r="B16" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="E16" s="11" t="n">
+      <c r="E16" s="10" t="n">
         <v>108</v>
       </c>
-      <c r="H16" s="11" t="n">
+      <c r="H16" s="10" t="n">
         <v>127</v>
       </c>
-      <c r="K16" s="11" t="n">
+      <c r="K16" s="10" t="n">
         <v>563</v>
       </c>
     </row>
     <row r="17" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A17" s="14" t="n"/>
-      <c r="B17" s="10" t="n">
+      <c r="A17" s="13" t="n"/>
+      <c r="B17" s="9" t="n">
         <v>754</v>
       </c>
       <c r="C17" s="4" t="n"/>
-      <c r="D17" s="14" t="n"/>
-      <c r="E17" s="10" t="n">
+      <c r="D17" s="13" t="n"/>
+      <c r="E17" s="9" t="n">
         <v>451</v>
       </c>
       <c r="F17" s="4" t="n"/>
-      <c r="G17" s="14" t="n"/>
-      <c r="H17" s="10" t="n">
+      <c r="G17" s="13" t="n"/>
+      <c r="H17" s="9" t="n">
         <v>920</v>
       </c>
       <c r="I17" s="4" t="n"/>
-      <c r="J17" s="14" t="n"/>
-      <c r="K17" s="10" t="n">
+      <c r="J17" s="13" t="n"/>
+      <c r="K17" s="9" t="n">
         <v>784</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A18" s="15" t="n"/>
+      <c r="A18" s="14" t="n"/>
       <c r="B18" s="7" t="n"/>
       <c r="C18" s="6" t="n"/>
-      <c r="D18" s="15" t="n"/>
+      <c r="D18" s="14" t="n"/>
       <c r="E18" s="7" t="n"/>
       <c r="F18" s="6" t="n"/>
-      <c r="G18" s="15" t="n"/>
+      <c r="G18" s="14" t="n"/>
       <c r="H18" s="7" t="n"/>
       <c r="I18" s="6" t="n"/>
-      <c r="J18" s="15" t="n"/>
+      <c r="J18" s="14" t="n"/>
       <c r="K18" s="7" t="n"/>
     </row>
     <row r="19" ht="20.25" customHeight="1">
@@ -2961,7 +2958,7 @@
       </c>
     </row>
     <row r="20" ht="20.25" customHeight="1">
-      <c r="A20" s="12" t="inlineStr">
+      <c r="A20" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2969,7 +2966,7 @@
       <c r="B20" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="D20" s="12" t="inlineStr">
+      <c r="D20" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2977,7 +2974,7 @@
       <c r="E20" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="G20" s="12" t="inlineStr">
+      <c r="G20" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2985,7 +2982,7 @@
       <c r="H20" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="J20" s="12" t="inlineStr">
+      <c r="J20" s="11" t="inlineStr">
         <is>
           <t>×</t>
         </is>
@@ -2995,51 +2992,51 @@
       </c>
     </row>
     <row r="21" ht="20.25" customHeight="1">
-      <c r="B21" s="9" t="n">
+      <c r="B21" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="E21" s="9" t="n">
+      <c r="E21" s="8" t="n">
         <v>108</v>
       </c>
-      <c r="H21" s="9" t="n">
+      <c r="H21" s="8" t="n">
         <v>127</v>
       </c>
-      <c r="K21" s="9" t="n">
+      <c r="K21" s="8" t="n">
         <v>563</v>
       </c>
     </row>
     <row r="22" ht="20.25" customHeight="1">
-      <c r="B22" s="11" t="n">
+      <c r="B22" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="E22" s="11" t="n">
+      <c r="E22" s="10" t="n">
         <v>108</v>
       </c>
-      <c r="H22" s="11" t="n">
+      <c r="H22" s="10" t="n">
         <v>127</v>
       </c>
-      <c r="K22" s="11" t="n">
+      <c r="K22" s="10" t="n">
         <v>563</v>
       </c>
     </row>
     <row r="23" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A23" s="14" t="n"/>
-      <c r="B23" s="10" t="n">
+      <c r="A23" s="13" t="n"/>
+      <c r="B23" s="9" t="n">
         <v>408</v>
       </c>
       <c r="C23" s="4" t="n"/>
-      <c r="D23" s="14" t="n"/>
-      <c r="E23" s="10" t="n">
+      <c r="D23" s="13" t="n"/>
+      <c r="E23" s="9" t="n">
         <v>468</v>
       </c>
       <c r="F23" s="4" t="n"/>
-      <c r="G23" s="14" t="n"/>
-      <c r="H23" s="10" t="n">
+      <c r="G23" s="13" t="n"/>
+      <c r="H23" s="9" t="n">
         <v>216</v>
       </c>
       <c r="I23" s="4" t="n"/>
-      <c r="J23" s="14" t="n"/>
-      <c r="K23" s="10" t="n">
+      <c r="J23" s="13" t="n"/>
+      <c r="K23" s="9" t="n">
         <v>418</v>
       </c>
     </row>
@@ -3056,371 +3053,351 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.140625" defaultRowHeight="21"/>
   <cols>
-    <col width="6.140625" customWidth="1" style="17" min="1" max="2"/>
-    <col width="2.85546875" customWidth="1" style="17" min="3" max="3"/>
-    <col width="6.140625" customWidth="1" style="17" min="4" max="5"/>
-    <col width="2.85546875" customWidth="1" style="17" min="6" max="6"/>
-    <col width="6.140625" customWidth="1" style="17" min="7" max="8"/>
-    <col width="2.85546875" customWidth="1" style="17" min="9" max="9"/>
-    <col width="6.140625" customWidth="1" style="17" min="10" max="11"/>
-    <col width="2.85546875" customWidth="1" style="17" min="12" max="12"/>
-    <col width="12.140625" customWidth="1" style="17" min="13" max="24"/>
-    <col width="12.140625" customWidth="1" style="17" min="25" max="16384"/>
+    <col width="6.140625" customWidth="1" style="16" min="1" max="2"/>
+    <col width="2.85546875" customWidth="1" style="16" min="3" max="3"/>
+    <col width="6.140625" customWidth="1" style="16" min="4" max="5"/>
+    <col width="2.85546875" customWidth="1" style="16" min="6" max="6"/>
+    <col width="6.140625" customWidth="1" style="16" min="7" max="8"/>
+    <col width="2.85546875" customWidth="1" style="16" min="9" max="9"/>
+    <col width="6.140625" customWidth="1" style="16" min="10" max="11"/>
+    <col width="2.85546875" customWidth="1" style="16" min="12" max="12"/>
+    <col width="12.140625" customWidth="1" style="16" min="13" max="26"/>
+    <col width="12.140625" customWidth="1" style="16" min="27" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" s="16" t="n">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="n">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="15" t="n">
+        <v>300</v>
+      </c>
+      <c r="B1" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D1" s="15" t="n">
+        <v>144</v>
+      </c>
+      <c r="E1" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="15" t="n">
+        <v>427</v>
+      </c>
+      <c r="H1" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="15" t="n">
+        <v>496</v>
+      </c>
+      <c r="K1" s="16" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" s="19" t="n"/>
+      <c r="B2" s="17" t="n"/>
+      <c r="D2" s="19" t="n"/>
+      <c r="E2" s="17" t="n"/>
+      <c r="G2" s="19" t="n"/>
+      <c r="H2" s="17" t="n"/>
+      <c r="J2" s="19" t="n"/>
+      <c r="K2" s="17" t="n"/>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" s="19" t="n"/>
+      <c r="B3" s="18" t="n"/>
+      <c r="D3" s="19" t="n"/>
+      <c r="E3" s="18" t="n"/>
+      <c r="G3" s="19" t="n"/>
+      <c r="H3" s="18" t="n"/>
+      <c r="J3" s="19" t="n"/>
+      <c r="K3" s="18" t="n"/>
+    </row>
+    <row r="4" ht="36" customHeight="1">
+      <c r="A4" s="18" t="n"/>
+      <c r="B4" s="18" t="n"/>
+      <c r="D4" s="18" t="n"/>
+      <c r="E4" s="18" t="n"/>
+      <c r="G4" s="18" t="n"/>
+      <c r="H4" s="18" t="n"/>
+      <c r="J4" s="18" t="n"/>
+      <c r="K4" s="18" t="n"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="15" t="n">
+        <v>252</v>
+      </c>
+      <c r="B5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>784</v>
+      </c>
+      <c r="E5" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" s="15" t="n">
+        <v>426</v>
+      </c>
+      <c r="H5" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="J5" s="15" t="n">
+        <v>264</v>
+      </c>
+      <c r="K5" s="16" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="19" t="n"/>
+      <c r="B6" s="17" t="n"/>
+      <c r="D6" s="19" t="n"/>
+      <c r="E6" s="17" t="n"/>
+      <c r="G6" s="19" t="n"/>
+      <c r="H6" s="17" t="n"/>
+      <c r="J6" s="19" t="n"/>
+      <c r="K6" s="17" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="19" t="n"/>
+      <c r="B7" s="18" t="n"/>
+      <c r="D7" s="19" t="n"/>
+      <c r="E7" s="18" t="n"/>
+      <c r="G7" s="19" t="n"/>
+      <c r="H7" s="18" t="n"/>
+      <c r="J7" s="19" t="n"/>
+      <c r="K7" s="18" t="n"/>
+    </row>
+    <row r="8" ht="36" customHeight="1">
+      <c r="A8" s="18" t="n"/>
+      <c r="B8" s="18" t="n"/>
+      <c r="D8" s="18" t="n"/>
+      <c r="E8" s="18" t="n"/>
+      <c r="G8" s="18" t="n"/>
+      <c r="H8" s="18" t="n"/>
+      <c r="J8" s="18" t="n"/>
+      <c r="K8" s="18" t="n"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="15" t="n">
+        <v>140</v>
+      </c>
+      <c r="B9" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="15" t="n">
+        <v>120</v>
+      </c>
+      <c r="E9" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="H9" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="n">
+      <c r="J9" s="15" t="n">
+        <v>560</v>
+      </c>
+      <c r="K9" s="16" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="19" t="n"/>
+      <c r="B10" s="17" t="n"/>
+      <c r="D10" s="19" t="n"/>
+      <c r="E10" s="17" t="n"/>
+      <c r="G10" s="19" t="n"/>
+      <c r="H10" s="17" t="n"/>
+      <c r="J10" s="19" t="n"/>
+      <c r="K10" s="17" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="19" t="n"/>
+      <c r="B11" s="18" t="n"/>
+      <c r="D11" s="19" t="n"/>
+      <c r="E11" s="18" t="n"/>
+      <c r="G11" s="19" t="n"/>
+      <c r="H11" s="18" t="n"/>
+      <c r="J11" s="19" t="n"/>
+      <c r="K11" s="18" t="n"/>
+    </row>
+    <row r="12" ht="36" customHeight="1">
+      <c r="A12" s="18" t="n"/>
+      <c r="B12" s="18" t="n"/>
+      <c r="D12" s="18" t="n"/>
+      <c r="E12" s="18" t="n"/>
+      <c r="G12" s="18" t="n"/>
+      <c r="H12" s="18" t="n"/>
+      <c r="J12" s="18" t="n"/>
+      <c r="K12" s="18" t="n"/>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" s="15" t="n">
+        <v>270</v>
+      </c>
+      <c r="B13" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="D13" s="15" t="n">
+        <v>294</v>
+      </c>
+      <c r="E13" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" s="15" t="n">
+        <v>276</v>
+      </c>
+      <c r="H13" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="J13" s="15" t="n">
+        <v>205</v>
+      </c>
+      <c r="K13" s="16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="19" t="n"/>
+      <c r="B14" s="17" t="n"/>
+      <c r="D14" s="19" t="n"/>
+      <c r="E14" s="17" t="n"/>
+      <c r="G14" s="19" t="n"/>
+      <c r="H14" s="17" t="n"/>
+      <c r="J14" s="19" t="n"/>
+      <c r="K14" s="17" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="19" t="n"/>
+      <c r="B15" s="18" t="n"/>
+      <c r="D15" s="19" t="n"/>
+      <c r="E15" s="18" t="n"/>
+      <c r="G15" s="19" t="n"/>
+      <c r="H15" s="18" t="n"/>
+      <c r="J15" s="19" t="n"/>
+      <c r="K15" s="18" t="n"/>
+    </row>
+    <row r="16" ht="36" customHeight="1">
+      <c r="A16" s="18" t="n"/>
+      <c r="B16" s="18" t="n"/>
+      <c r="D16" s="18" t="n"/>
+      <c r="E16" s="18" t="n"/>
+      <c r="G16" s="18" t="n"/>
+      <c r="H16" s="18" t="n"/>
+      <c r="J16" s="18" t="n"/>
+      <c r="K16" s="18" t="n"/>
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" s="15" t="n">
+        <v>150</v>
+      </c>
+      <c r="B17" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>26</v>
+      </c>
+      <c r="E17" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="n">
+      <c r="G17" s="15" t="n">
+        <v>322</v>
+      </c>
+      <c r="H17" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="J17" s="15" t="n">
+        <v>158</v>
+      </c>
+      <c r="K17" s="16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="19" t="n"/>
+      <c r="B18" s="17" t="n"/>
+      <c r="D18" s="19" t="n"/>
+      <c r="E18" s="17" t="n"/>
+      <c r="G18" s="19" t="n"/>
+      <c r="H18" s="17" t="n"/>
+      <c r="J18" s="19" t="n"/>
+      <c r="K18" s="17" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="19" t="n"/>
+      <c r="B19" s="18" t="n"/>
+      <c r="D19" s="19" t="n"/>
+      <c r="E19" s="18" t="n"/>
+      <c r="G19" s="19" t="n"/>
+      <c r="H19" s="18" t="n"/>
+      <c r="J19" s="19" t="n"/>
+      <c r="K19" s="18" t="n"/>
+    </row>
+    <row r="20" ht="36" customHeight="1">
+      <c r="A20" s="18" t="n"/>
+      <c r="B20" s="18" t="n"/>
+      <c r="D20" s="18" t="n"/>
+      <c r="E20" s="18" t="n"/>
+      <c r="G20" s="18" t="n"/>
+      <c r="H20" s="18" t="n"/>
+      <c r="J20" s="18" t="n"/>
+      <c r="K20" s="18" t="n"/>
+    </row>
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" s="15" t="n">
+        <v>268</v>
+      </c>
+      <c r="B21" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="15" t="n">
+        <v>72</v>
+      </c>
+      <c r="E21" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G21" s="15" t="n">
+        <v>138</v>
+      </c>
+      <c r="H21" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="J21" s="15" t="n">
+        <v>290</v>
+      </c>
+      <c r="K21" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="H1" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="J1" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="K1" s="3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="20" t="n"/>
-      <c r="B2" s="18" t="n"/>
-      <c r="D2" s="20" t="n"/>
-      <c r="E2" s="18" t="n"/>
-      <c r="G2" s="20" t="n"/>
-      <c r="H2" s="18" t="n"/>
-      <c r="J2" s="20" t="n"/>
-      <c r="K2" s="18" t="n"/>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="20" t="n"/>
-      <c r="B3" s="19" t="n"/>
-      <c r="D3" s="20" t="n"/>
-      <c r="E3" s="19" t="n"/>
-      <c r="G3" s="20" t="n"/>
-      <c r="H3" s="19" t="n"/>
-      <c r="J3" s="20" t="n"/>
-      <c r="K3" s="19" t="n"/>
-    </row>
-    <row r="4" ht="20.25" customHeight="1">
-      <c r="A4" s="19" t="n"/>
-      <c r="B4" s="19" t="n"/>
-      <c r="C4" s="17" t="n"/>
-      <c r="D4" s="19" t="n"/>
-      <c r="E4" s="19" t="n"/>
-      <c r="F4" s="17" t="n"/>
-      <c r="G4" s="19" t="n"/>
-      <c r="H4" s="19" t="n"/>
-      <c r="I4" s="17" t="n"/>
-      <c r="J4" s="19" t="n"/>
-      <c r="K4" s="19" t="n"/>
-      <c r="L4" s="17" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="D5" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G5" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="J5" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="20" t="n"/>
-      <c r="B6" s="18" t="n"/>
-      <c r="D6" s="20" t="n"/>
-      <c r="E6" s="18" t="n"/>
-      <c r="G6" s="20" t="n"/>
-      <c r="H6" s="18" t="n"/>
-      <c r="J6" s="20" t="n"/>
-      <c r="K6" s="18" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="20" t="n"/>
-      <c r="B7" s="19" t="n"/>
-      <c r="D7" s="20" t="n"/>
-      <c r="E7" s="19" t="n"/>
-      <c r="G7" s="20" t="n"/>
-      <c r="H7" s="19" t="n"/>
-      <c r="J7" s="20" t="n"/>
-      <c r="K7" s="19" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="19" t="n"/>
-      <c r="B8" s="19" t="n"/>
-      <c r="C8" s="17" t="n"/>
-      <c r="D8" s="19" t="n"/>
-      <c r="E8" s="19" t="n"/>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="19" t="n"/>
-      <c r="H8" s="19" t="n"/>
-      <c r="I8" s="17" t="n"/>
-      <c r="J8" s="19" t="n"/>
-      <c r="K8" s="19" t="n"/>
-      <c r="L8" s="17" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="D9" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="J9" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="K9" s="3" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="20" t="n"/>
-      <c r="B10" s="18" t="n"/>
-      <c r="D10" s="20" t="n"/>
-      <c r="E10" s="18" t="n"/>
-      <c r="G10" s="20" t="n"/>
-      <c r="H10" s="18" t="n"/>
-      <c r="J10" s="20" t="n"/>
-      <c r="K10" s="18" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="20" t="n"/>
-      <c r="B11" s="19" t="n"/>
-      <c r="D11" s="20" t="n"/>
-      <c r="E11" s="19" t="n"/>
-      <c r="G11" s="20" t="n"/>
-      <c r="H11" s="19" t="n"/>
-      <c r="J11" s="20" t="n"/>
-      <c r="K11" s="19" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="19" t="n"/>
-      <c r="B12" s="19" t="n"/>
-      <c r="C12" s="17" t="n"/>
-      <c r="D12" s="19" t="n"/>
-      <c r="E12" s="19" t="n"/>
-      <c r="F12" s="17" t="n"/>
-      <c r="G12" s="19" t="n"/>
-      <c r="H12" s="19" t="n"/>
-      <c r="I12" s="17" t="n"/>
-      <c r="J12" s="19" t="n"/>
-      <c r="K12" s="19" t="n"/>
-      <c r="L12" s="17" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D13" s="16" t="n">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="G13" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="H13" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="J13" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="K13" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="20" t="n"/>
-      <c r="B14" s="18" t="n"/>
-      <c r="D14" s="20" t="n"/>
-      <c r="E14" s="18" t="n"/>
-      <c r="G14" s="20" t="n"/>
-      <c r="H14" s="18" t="n"/>
-      <c r="J14" s="20" t="n"/>
-      <c r="K14" s="18" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="20" t="n"/>
-      <c r="B15" s="19" t="n"/>
-      <c r="D15" s="20" t="n"/>
-      <c r="E15" s="19" t="n"/>
-      <c r="G15" s="20" t="n"/>
-      <c r="H15" s="19" t="n"/>
-      <c r="J15" s="20" t="n"/>
-      <c r="K15" s="19" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="19" t="n"/>
-      <c r="B16" s="19" t="n"/>
-      <c r="C16" s="17" t="n"/>
-      <c r="D16" s="19" t="n"/>
-      <c r="E16" s="19" t="n"/>
-      <c r="F16" s="17" t="n"/>
-      <c r="G16" s="19" t="n"/>
-      <c r="H16" s="19" t="n"/>
-      <c r="I16" s="17" t="n"/>
-      <c r="J16" s="19" t="n"/>
-      <c r="K16" s="19" t="n"/>
-      <c r="L16" s="17" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="D17" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="E17" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G17" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="H17" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="J17" s="16" t="n">
-        <v>7</v>
-      </c>
-      <c r="K17" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="20" t="n"/>
-      <c r="B18" s="18" t="n"/>
-      <c r="D18" s="20" t="n"/>
-      <c r="E18" s="18" t="n"/>
-      <c r="G18" s="20" t="n"/>
-      <c r="H18" s="18" t="n"/>
-      <c r="J18" s="20" t="n"/>
-      <c r="K18" s="18" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="20" t="n"/>
-      <c r="B19" s="19" t="n"/>
-      <c r="D19" s="20" t="n"/>
-      <c r="E19" s="19" t="n"/>
-      <c r="G19" s="20" t="n"/>
-      <c r="H19" s="19" t="n"/>
-      <c r="J19" s="20" t="n"/>
-      <c r="K19" s="19" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="19" t="n"/>
-      <c r="B20" s="19" t="n"/>
-      <c r="C20" s="17" t="n"/>
-      <c r="D20" s="19" t="n"/>
-      <c r="E20" s="19" t="n"/>
-      <c r="F20" s="17" t="n"/>
-      <c r="G20" s="19" t="n"/>
-      <c r="H20" s="19" t="n"/>
-      <c r="I20" s="17" t="n"/>
-      <c r="J20" s="19" t="n"/>
-      <c r="K20" s="19" t="n"/>
-      <c r="L20" s="17" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="16" t="n">
-        <v>9</v>
-      </c>
-      <c r="B21" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D21" s="16" t="n">
-        <v>9</v>
-      </c>
-      <c r="E21" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G21" s="16" t="n">
-        <v>6</v>
-      </c>
-      <c r="H21" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="J21" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="K21" s="3" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="22">
-      <c r="A22" s="20" t="n"/>
-      <c r="B22" s="18" t="n"/>
-      <c r="D22" s="20" t="n"/>
-      <c r="E22" s="18" t="n"/>
-      <c r="G22" s="20" t="n"/>
-      <c r="H22" s="18" t="n"/>
-      <c r="J22" s="20" t="n"/>
-      <c r="K22" s="18" t="n"/>
+      <c r="A22" s="19" t="n"/>
+      <c r="B22" s="17" t="n"/>
+      <c r="D22" s="19" t="n"/>
+      <c r="E22" s="17" t="n"/>
+      <c r="G22" s="19" t="n"/>
+      <c r="H22" s="17" t="n"/>
+      <c r="J22" s="19" t="n"/>
+      <c r="K22" s="17" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="20" t="n"/>
-      <c r="B23" s="19" t="n"/>
-      <c r="D23" s="20" t="n"/>
-      <c r="E23" s="19" t="n"/>
-      <c r="G23" s="20" t="n"/>
-      <c r="H23" s="19" t="n"/>
-      <c r="J23" s="20" t="n"/>
-      <c r="K23" s="19" t="n"/>
+      <c r="A23" s="19" t="n"/>
+      <c r="B23" s="18" t="n"/>
+      <c r="D23" s="19" t="n"/>
+      <c r="E23" s="18" t="n"/>
+      <c r="G23" s="19" t="n"/>
+      <c r="H23" s="18" t="n"/>
+      <c r="J23" s="19" t="n"/>
+      <c r="K23" s="18" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.5511811023622047" bottom="0.5511811023622047" header="0.3149606299212598" footer="0.3149606299212598"/>

</xml_diff>